<commit_message>
Adds remaining non-Orleans test data
</commit_message>
<xml_diff>
--- a/ACVP-time-data.xlsx
+++ b/ACVP-time-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctc\Documents\ACVP\gen-val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1E525B91-1907-402A-B904-64FD5496C9B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4860C552-C1F1-41E8-814D-BB1902EB7E6C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" xr2:uid="{C4ACC8D3-7241-42A3-8C9D-B3AF3FAEEB3A}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Algo</t>
   </si>
   <si>
-    <t>No Server, No Orleans</t>
-  </si>
-  <si>
     <t>AES-CCM</t>
   </si>
   <si>
@@ -282,7 +279,13 @@
     <t>Total (for both)</t>
   </si>
   <si>
-    <t>No Server, Orleans: 2 Silos, 4 Cores ea, 4GB RAM ea</t>
+    <t>0:15:46:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Server, No Orleans, 4 Cores, </t>
+  </si>
+  <si>
+    <t>No Server, Orleans: 2 Silos, 4 Cores ea, 4GB RAM ea (Potential large resource sharing)</t>
   </si>
 </sst>
 </file>
@@ -401,13 +404,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,15 +727,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E10E21-FE83-4458-90DB-272C076FA706}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
   </cols>
@@ -741,14 +744,14 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="15"/>
       <c r="F1" s="5"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -756,16 +759,16 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="D2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7"/>
@@ -773,7 +776,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3">
         <v>3.3096064814814815E-4</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>2.0844907407407411E-5</v>
@@ -809,7 +812,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>3.3798611111111112E-4</v>
@@ -827,7 +830,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>3.4018518518518518E-4</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
         <v>3.3868055555555556E-4</v>
@@ -863,7 +866,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>1.6018518518518518E-5</v>
@@ -881,7 +884,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>3.2599537037037037E-4</v>
@@ -899,7 +902,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>1.3287037037037035E-5</v>
@@ -917,7 +920,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>3.3040509259259259E-4</v>
@@ -935,7 +938,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>3.1105324074074076E-4</v>
@@ -953,7 +956,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3.3939814814814813E-4</v>
@@ -971,7 +974,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3">
         <v>1.3761574074074072E-5</v>
@@ -989,12 +992,12 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="9">
         <v>1.8982638888888887E-4</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="13">
         <v>1.6875E-5</v>
       </c>
       <c r="D15" s="9">
@@ -1009,7 +1012,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>3.4976851851851853E-5</v>
@@ -1027,12 +1030,12 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="9">
         <v>2.2974537037037037E-5</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="13">
         <v>1.1006944444444445E-5</v>
       </c>
       <c r="D17" s="9">
@@ -1047,7 +1050,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="3">
         <v>1.7835648148148147E-5</v>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3">
         <v>1.5555555555555552E-5</v>
@@ -1083,12 +1086,12 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="9">
         <v>3.659722222222222E-5</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="13">
         <v>1.0185185185185185E-5</v>
       </c>
       <c r="D20" s="9">
@@ -1103,7 +1106,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3">
         <v>3.021168981481481E-3</v>
@@ -1121,7 +1124,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <v>4.9186990740740739E-2</v>
@@ -1139,7 +1142,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3">
         <v>0.13514511574074076</v>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
         <v>3.5283726851851847E-2</v>
@@ -1175,12 +1178,12 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="9">
         <v>4.4421296296296292E-2</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <v>1.0532407407407406E-5</v>
       </c>
       <c r="D25" s="9">
@@ -1195,7 +1198,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3">
         <v>6.1760648148148148E-3</v>
@@ -1213,7 +1216,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3">
         <v>3.8289930555555555E-3</v>
@@ -1231,7 +1234,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3">
         <v>2.1706365740740741E-2</v>
@@ -1249,12 +1252,12 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="9">
         <v>5.5348182870370376E-2</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="13">
         <v>1.0451388888888889E-5</v>
       </c>
       <c r="D29" s="9">
@@ -1269,7 +1272,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3">
         <v>1.1435185185185186E-5</v>
@@ -1287,7 +1290,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="3">
         <v>1.1481481481481482E-5</v>
@@ -1305,7 +1308,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3">
         <v>1.9062499999999999E-5</v>
@@ -1323,12 +1326,12 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="9">
         <v>1.3310185185185184E-5</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="13">
         <v>9.8495370370370364E-6</v>
       </c>
       <c r="D33" s="9">
@@ -1343,7 +1346,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="3">
         <v>1.5081018518518518E-5</v>
@@ -1361,7 +1364,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3">
         <v>1.511574074074074E-5</v>
@@ -1379,7 +1382,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="3">
         <v>1.4895833333333334E-5</v>
@@ -1397,7 +1400,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="3">
         <v>2.0196759259259262E-5</v>
@@ -1415,7 +1418,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="3">
         <v>2.0520833333333339E-5</v>
@@ -1433,7 +1436,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3">
         <v>2.0266203703703701E-5</v>
@@ -1451,7 +1454,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="3">
         <v>2.0150462962962964E-5</v>
@@ -1469,7 +1472,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="3">
         <v>3.2291666666666668E-5</v>
@@ -1487,7 +1490,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="3">
         <v>3.0810185185185184E-5</v>
@@ -1505,7 +1508,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="3">
         <v>2.8043981481481482E-5</v>
@@ -1523,12 +1526,12 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="9">
         <v>2.6076388888888891E-5</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="13">
         <v>1.0752314814814814E-5</v>
       </c>
       <c r="D44" s="9">
@@ -1543,13 +1546,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>7.2380208333333342E-3</v>
       </c>
       <c r="C45" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>5.8207175925925928E-4</v>
       </c>
       <c r="D45" s="3">
         <v>8.4000347222222219E-3</v>
@@ -1561,13 +1564,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.344675925925926E-4</v>
       </c>
       <c r="C46" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>8.2638888888888877E-5</v>
       </c>
       <c r="D46" s="3">
         <v>2.4920138888888892E-4</v>
@@ -1579,13 +1582,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C47" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>9.3884837962962958E-3</v>
+      </c>
+      <c r="C47" s="13">
+        <v>1.1142361111111112E-4</v>
       </c>
       <c r="D47" s="9">
         <v>1.7745752314814813E-2</v>
@@ -1599,13 +1602,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>3.6736111111111104E-5</v>
       </c>
       <c r="C48" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>3.3819444444444446E-5</v>
       </c>
       <c r="D48" s="3">
         <v>1.4815972222222224E-4</v>
@@ -1617,13 +1620,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.241898148148148E-5</v>
       </c>
       <c r="C49" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0104166666666667E-5</v>
       </c>
       <c r="D49" s="3">
         <v>7.6481481481481477E-5</v>
@@ -1635,13 +1638,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.2140046296296297E-4</v>
       </c>
       <c r="C50" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>2.1574074074074074E-5</v>
       </c>
       <c r="D50" s="3">
         <v>1.7368055555555553E-4</v>
@@ -1653,13 +1656,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>7.5628472222222232E-4</v>
       </c>
       <c r="C51" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>3.0844907407407404E-5</v>
       </c>
       <c r="D51" s="3">
         <v>9.2841435185185182E-4</v>
@@ -1671,13 +1674,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>7.1494212962962961E-4</v>
       </c>
       <c r="C52" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0046296296296295E-5</v>
       </c>
       <c r="D52" s="3">
         <v>1.0024537037037038E-3</v>
@@ -1689,13 +1692,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.3310185185185184E-5</v>
       </c>
       <c r="C53" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0694444444444444E-5</v>
       </c>
       <c r="D53" s="3">
         <v>7.6956018518518506E-5</v>
@@ -1707,13 +1710,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.7314814814814813E-5</v>
       </c>
       <c r="C54" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0578703703703704E-5</v>
       </c>
       <c r="D54" s="3">
         <v>1.35E-4</v>
@@ -1725,13 +1728,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C55" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>3.7696759259259257E-5</v>
+      </c>
+      <c r="C55" s="13">
+        <v>1.0011574074074073E-5</v>
       </c>
       <c r="D55" s="9">
         <v>7.657407407407408E-5</v>
@@ -1745,13 +1748,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>4.9097222222222219E-5</v>
       </c>
       <c r="C56" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1817129629629629E-5</v>
       </c>
       <c r="D56" s="3">
         <v>8.4942129629629636E-5</v>
@@ -1763,13 +1766,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>7.4361111111111112E-4</v>
       </c>
       <c r="C57" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.2384259259259259E-5</v>
       </c>
       <c r="D57" s="3">
         <v>1.4125462962962963E-3</v>
@@ -1781,13 +1784,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>6.5392361111111109E-4</v>
       </c>
       <c r="C58" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1018518518518517E-5</v>
       </c>
       <c r="D58" s="3">
         <v>1.1114583333333334E-3</v>
@@ -1799,13 +1802,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C59" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>3.3207175925925922E-4</v>
+      </c>
+      <c r="C59" s="13">
+        <v>1.0856481481481481E-5</v>
       </c>
       <c r="D59" s="9">
         <v>6.2337962962962965E-4</v>
@@ -1819,13 +1822,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1748842592592593E-4</v>
       </c>
       <c r="C60" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0393518518518519E-5</v>
       </c>
       <c r="D60" s="3">
         <v>1.1196759259259261E-3</v>
@@ -1837,13 +1840,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.182840277777778E-2</v>
       </c>
       <c r="C61" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1238425925925927E-5</v>
       </c>
       <c r="D61" s="3">
         <v>2.4111747685185186E-2</v>
@@ -1855,13 +1858,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>0.12474755787037035</v>
       </c>
       <c r="C62" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1562500000000002E-5</v>
       </c>
       <c r="D62" s="3">
         <v>0.15535005787037037</v>
@@ -1873,13 +1876,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.9853796296296296E-2</v>
       </c>
       <c r="C63" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.3067129629629629E-5</v>
       </c>
       <c r="D63" s="3">
         <v>2.1028321759259259E-2</v>
@@ -1891,13 +1894,13 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B64" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>3.4185648148148148E-3</v>
       </c>
       <c r="C64" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>9.9189814814814818E-6</v>
       </c>
       <c r="D64" s="3">
         <v>7.8845601851851854E-3</v>
@@ -1909,13 +1912,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C65" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>6.9067789351851858E-2</v>
+      </c>
+      <c r="C65" s="13">
+        <v>1.1388888888888891E-5</v>
       </c>
       <c r="D65" s="9">
         <v>8.5467986111111116E-2</v>
@@ -1929,13 +1932,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>3.4432870370370368E-4</v>
       </c>
       <c r="C66" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1597222222222223E-5</v>
       </c>
       <c r="D66" s="3">
         <v>1.8459953703703705E-3</v>
@@ -1947,13 +1950,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>6.9495370370370371E-4</v>
       </c>
       <c r="C67" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.116898148148148E-5</v>
       </c>
       <c r="D67" s="3">
         <v>1.6427777777777779E-3</v>
@@ -1965,13 +1968,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C68" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>6.9812500000000007E-4</v>
+      </c>
+      <c r="C68" s="13">
+        <v>1.3101851851851852E-5</v>
       </c>
       <c r="D68" s="9">
         <v>9.9212962962962948E-4</v>
@@ -1985,13 +1988,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>6.5759259259259254E-4</v>
       </c>
       <c r="C69" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0902777777777777E-5</v>
       </c>
       <c r="D69" s="3">
         <v>1.0860532407407407E-3</v>
@@ -2003,13 +2006,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B70" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1760416666666666E-3</v>
       </c>
       <c r="C70" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1516203703703702E-5</v>
       </c>
       <c r="D70" s="3">
         <v>1.4934722222222222E-3</v>
@@ -2021,13 +2024,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>6.0643518518518522E-4</v>
       </c>
       <c r="C71" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0833333333333335E-5</v>
       </c>
       <c r="D71" s="3">
         <v>9.7005787037037026E-4</v>
@@ -2039,13 +2042,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>6.8046296296296301E-4</v>
       </c>
       <c r="C72" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D72" s="3">
         <v>9.7078703703703704E-4</v>
@@ -2057,13 +2060,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B73" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>5.9113425925925924E-4</v>
       </c>
       <c r="C73" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0868055555555556E-5</v>
       </c>
       <c r="D73" s="3">
         <v>8.5445601851851861E-4</v>
@@ -2075,13 +2078,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B74" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>9.0486111111111106E-4</v>
       </c>
       <c r="C74" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1574074074074073E-5</v>
       </c>
       <c r="D74" s="3">
         <v>1.6077430555555556E-3</v>
@@ -2093,13 +2096,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>9.9563657407407413E-4</v>
       </c>
       <c r="C75" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.116898148148148E-5</v>
       </c>
       <c r="D75" s="3">
         <v>1.7817245370370372E-3</v>
@@ -2111,13 +2114,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>8.961921296296297E-4</v>
       </c>
       <c r="C76" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0798611111111113E-5</v>
       </c>
       <c r="D76" s="3">
         <v>1.2020601851851851E-3</v>
@@ -2129,13 +2132,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.2719907407407405E-5</v>
       </c>
       <c r="C77" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.0902777777777777E-5</v>
       </c>
       <c r="D77" s="3">
         <v>7.6435185185185189E-5</v>
@@ -2147,13 +2150,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B78" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>5.6252314814814804E-4</v>
       </c>
       <c r="C78" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1122685185185185E-5</v>
       </c>
       <c r="D78" s="3">
         <v>1.1562037037037038E-3</v>
@@ -2165,13 +2168,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B79" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>2.5046296296296299E-5</v>
       </c>
       <c r="C79" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.1620370370370372E-5</v>
       </c>
       <c r="D79" s="3">
         <v>7.9652777777777773E-5</v>
@@ -2183,13 +2186,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B80" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>7.2937499999999999E-4</v>
       </c>
       <c r="C80" s="3">
-        <v>1.5399189814814815E-3</v>
+        <v>1.070601851851852E-5</v>
       </c>
       <c r="D80" s="3">
         <v>1.0278587962962962E-3</v>
@@ -2201,13 +2204,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="9">
-        <v>1.5399189814814815E-3</v>
-      </c>
-      <c r="C81" s="15">
-        <v>1.5399189814814815E-3</v>
+        <v>6.4694444444444445E-4</v>
+      </c>
+      <c r="C81" s="13">
+        <v>1.1539351851851851E-5</v>
       </c>
       <c r="D81" s="9">
         <v>9.7200231481481486E-4</v>
@@ -2221,12 +2224,14 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B82" s="5"/>
       <c r="C82" s="6"/>
       <c r="D82" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="5"/>

</xml_diff>

<commit_message>
updated spreadsheet to indicate max concurrency from previous orleans test
</commit_message>
<xml_diff>
--- a/ACVP-time-data.xlsx
+++ b/ACVP-time-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctc\Documents\ACVP\gen-val\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\gitLab\gen-val\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4860C552-C1F1-41E8-814D-BB1902EB7E6C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CA839F2-D228-4CC6-B638-4E23115005C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" xr2:uid="{C4ACC8D3-7241-42A3-8C9D-B3AF3FAEEB3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18876" windowHeight="7056" xr2:uid="{C4ACC8D3-7241-42A3-8C9D-B3AF3FAEEB3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -285,7 +285,7 @@
     <t xml:space="preserve">No Server, No Orleans, 4 Cores, </t>
   </si>
   <si>
-    <t>No Server, Orleans: 2 Silos, 4 Cores ea, 4GB RAM ea (Potential large resource sharing)</t>
+    <t>No Server, Orleans: 2 Silos, 4 Cores ea, 4GB RAM ea (Potential large resource sharing - "1" max limited concurrency)</t>
   </si>
 </sst>
 </file>
@@ -728,19 +728,19 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>81</v>
@@ -774,7 +774,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -792,7 +792,7 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -846,7 +846,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -882,7 +882,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -918,7 +918,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -936,7 +936,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -954,7 +954,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -990,7 +990,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1010,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>42</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
@@ -1196,7 +1196,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>29</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>41</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>45</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1690,7 +1690,7 @@
       </c>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>53</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
@@ -1820,7 +1820,7 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>61</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>64</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>77</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
     </row>

</xml_diff>